<commit_message>
Se concentro en el diagrama los modulos
Se concentro en el diagrama los módulos web
</commit_message>
<xml_diff>
--- a/00-Documentacion/ConcentradoDeModulosWeb.xlsx
+++ b/00-Documentacion/ConcentradoDeModulosWeb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9D9D14-DD6A-46B1-BE14-8F87BFB0B02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93EBE94-3C4A-481D-A779-599D683785AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02C913EA-5EF7-442D-8608-919950013EE6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{02C913EA-5EF7-442D-8608-919950013EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Portal_v2" sheetId="1" r:id="rId1"/>
@@ -1063,7 +1063,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1095,6 +1095,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1150,7 +1157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1169,6 +1176,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,7 +1496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D3A08E-BEB8-41FC-A18B-BA35F87E4739}">
   <dimension ref="A1:O214"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1775,12 +1788,12 @@
       <c r="A24">
         <v>3</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C25" s="8"/>
@@ -1789,11 +1802,12 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
       <c r="C27" s="4" t="s">
         <v>30</v>
       </c>
@@ -1805,6 +1819,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
       <c r="C28" s="4" t="s">
         <v>31</v>
       </c>
@@ -1816,7 +1831,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1881,16 +1896,17 @@
       <c r="A36">
         <v>5</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="17"/>
       <c r="C38" s="4" t="s">
         <v>49</v>
       </c>
@@ -1899,6 +1915,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
       <c r="E39" s="4" t="s">
         <v>50</v>
       </c>
@@ -1910,6 +1927,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="17"/>
       <c r="E40" s="4" t="s">
         <v>51</v>
       </c>
@@ -1921,6 +1939,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="17"/>
       <c r="C41" s="4" t="s">
         <v>70</v>
       </c>
@@ -1929,6 +1948,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="17"/>
       <c r="E42" s="4" t="s">
         <v>71</v>
       </c>
@@ -1940,6 +1960,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="17"/>
       <c r="E43" s="4" t="s">
         <v>72</v>
       </c>
@@ -1951,11 +1972,12 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="17"/>
       <c r="C45" s="4" t="s">
         <v>74</v>
       </c>
@@ -1964,6 +1986,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="17"/>
       <c r="E46" s="4" t="s">
         <v>76</v>
       </c>
@@ -2019,16 +2042,17 @@
       <c r="A51">
         <v>6</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="17"/>
       <c r="C53" s="4" t="s">
         <v>81</v>
       </c>
@@ -2037,6 +2061,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="17"/>
       <c r="E54" s="4" t="s">
         <v>82</v>
       </c>
@@ -2048,6 +2073,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="17"/>
       <c r="E55" s="4" t="s">
         <v>83</v>
       </c>
@@ -2059,6 +2085,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="17"/>
       <c r="C56" s="4" t="s">
         <v>84</v>
       </c>
@@ -2067,6 +2094,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="17"/>
       <c r="E57" s="4" t="s">
         <v>86</v>
       </c>
@@ -2078,6 +2106,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="17"/>
       <c r="E58" s="4" t="s">
         <v>87</v>
       </c>
@@ -2089,7 +2118,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="16" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2525,7 +2554,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="16" t="s">
         <v>125</v>
       </c>
       <c r="H102" t="s">
@@ -2533,7 +2562,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="12" t="s">
+      <c r="B103" s="14" t="s">
         <v>235</v>
       </c>
       <c r="H103" t="s">
@@ -2541,7 +2570,7 @@
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B104" s="12" t="s">
+      <c r="B104" s="14" t="s">
         <v>236</v>
       </c>
       <c r="H104" t="s">
@@ -2549,7 +2578,7 @@
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="16" t="s">
         <v>261</v>
       </c>
       <c r="H105" t="s">
@@ -2694,12 +2723,12 @@
       <c r="A122">
         <v>7</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="B122" s="15" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="16" t="s">
         <v>148</v>
       </c>
       <c r="H123" t="s">
@@ -2707,7 +2736,7 @@
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="16" t="s">
         <v>149</v>
       </c>
       <c r="H124" t="s">
@@ -2715,11 +2744,12 @@
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="16" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="17"/>
       <c r="C126" s="4" t="s">
         <v>157</v>
       </c>
@@ -2731,6 +2761,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="17"/>
       <c r="C127" s="4" t="s">
         <v>158</v>
       </c>
@@ -2742,6 +2773,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="17"/>
       <c r="C128" s="4" t="s">
         <v>159</v>
       </c>
@@ -2753,6 +2785,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="17"/>
       <c r="C129" s="4" t="s">
         <v>160</v>
       </c>
@@ -2764,11 +2797,12 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="16" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="17"/>
       <c r="C131" s="4" t="s">
         <v>171</v>
       </c>
@@ -2780,6 +2814,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="17"/>
       <c r="C132" s="4" t="s">
         <v>172</v>
       </c>
@@ -2791,6 +2826,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="17"/>
       <c r="C133" s="4" t="s">
         <v>173</v>
       </c>
@@ -2802,6 +2838,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="17"/>
       <c r="C134" s="4" t="s">
         <v>174</v>
       </c>
@@ -2813,6 +2850,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="17"/>
       <c r="C135" s="4" t="s">
         <v>175</v>
       </c>
@@ -2824,6 +2862,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="17"/>
       <c r="C136" s="4" t="s">
         <v>176</v>
       </c>
@@ -2835,6 +2874,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="17"/>
       <c r="C137" s="4" t="s">
         <v>177</v>
       </c>
@@ -2849,12 +2889,12 @@
       <c r="A138">
         <v>8</v>
       </c>
-      <c r="B138" s="7" t="s">
+      <c r="B138" s="15" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="16" t="s">
         <v>179</v>
       </c>
       <c r="H139" t="s">
@@ -2862,7 +2902,7 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="16" t="s">
         <v>180</v>
       </c>
       <c r="H140" t="s">
@@ -2870,7 +2910,7 @@
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H141" t="s">
@@ -2878,7 +2918,7 @@
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="16" t="s">
         <v>182</v>
       </c>
       <c r="H142" t="s">
@@ -2886,7 +2926,7 @@
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="16" t="s">
         <v>183</v>
       </c>
       <c r="H143" t="s">
@@ -2894,7 +2934,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="16" t="s">
         <v>184</v>
       </c>
       <c r="H144" t="s">
@@ -3002,7 +3042,7 @@
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="16" t="s">
         <v>237</v>
       </c>
       <c r="H154" t="s">
@@ -3010,7 +3050,7 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="16" t="s">
         <v>219</v>
       </c>
       <c r="H155" t="s">
@@ -3073,7 +3113,7 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="16" t="s">
         <v>225</v>
       </c>
       <c r="H161" t="s">
@@ -3084,12 +3124,12 @@
       <c r="A162">
         <v>3</v>
       </c>
-      <c r="B162" s="7" t="s">
+      <c r="B162" s="15" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="16" t="s">
         <v>201</v>
       </c>
       <c r="H163" t="s">
@@ -3097,7 +3137,7 @@
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="16" t="s">
         <v>202</v>
       </c>
       <c r="H164" t="s">
@@ -3132,7 +3172,7 @@
       <c r="C168" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D168" s="4" t="s">
+      <c r="D168" s="16" t="s">
         <v>281</v>
       </c>
       <c r="H168" t="s">
@@ -3182,7 +3222,7 @@
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B172" s="12" t="s">
+      <c r="B172" s="14" t="s">
         <v>287</v>
       </c>
       <c r="H172" t="s">
@@ -3243,7 +3283,7 @@
       <c r="C177" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="D177" s="12" t="s">
+      <c r="D177" s="14" t="s">
         <v>244</v>
       </c>
       <c r="H177" t="s">
@@ -3262,7 +3302,7 @@
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="16" t="s">
         <v>294</v>
       </c>
       <c r="H179" t="s">
@@ -3273,7 +3313,7 @@
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B180" s="4" t="s">
+      <c r="B180" s="16" t="s">
         <v>295</v>
       </c>
       <c r="H180" t="s">
@@ -3379,10 +3419,10 @@
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C189" s="4" t="s">
+      <c r="C189" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="D189" s="4" t="s">
+      <c r="D189" s="16" t="s">
         <v>266</v>
       </c>
       <c r="H189" t="s">
@@ -3423,10 +3463,10 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C193" s="4" t="s">
+      <c r="C193" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="D193" s="4" t="s">
+      <c r="D193" s="16" t="s">
         <v>263</v>
       </c>
       <c r="H193" t="s">
@@ -3548,12 +3588,12 @@
       <c r="A202">
         <v>1</v>
       </c>
-      <c r="B202" s="7" t="s">
+      <c r="B202" s="15" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B203" s="12" t="s">
+      <c r="B203" s="14" t="s">
         <v>311</v>
       </c>
       <c r="H203" t="s">
@@ -3564,7 +3604,7 @@
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B204" s="12" t="s">
+      <c r="B204" s="14" t="s">
         <v>312</v>
       </c>
       <c r="H204" t="s">
@@ -3572,7 +3612,7 @@
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B205" s="12" t="s">
+      <c r="B205" s="14" t="s">
         <v>321</v>
       </c>
       <c r="H205" t="s">
@@ -3580,7 +3620,7 @@
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B206" s="12" t="s">
+      <c r="B206" s="14" t="s">
         <v>323</v>
       </c>
       <c r="H206" t="s">
@@ -3588,7 +3628,7 @@
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B207" s="12" t="s">
+      <c r="B207" s="14" t="s">
         <v>324</v>
       </c>
       <c r="H207" t="s">
@@ -3596,7 +3636,7 @@
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B208" s="12" t="s">
+      <c r="B208" s="14" t="s">
         <v>325</v>
       </c>
       <c r="H208" t="s">
@@ -3604,7 +3644,7 @@
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B209" s="12" t="s">
+      <c r="B209" s="14" t="s">
         <v>326</v>
       </c>
       <c r="H209" t="s">
@@ -3612,7 +3652,7 @@
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B210" s="12" t="s">
+      <c r="B210" s="14" t="s">
         <v>327</v>
       </c>
       <c r="H210" t="s">
@@ -3620,7 +3660,7 @@
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B211" s="12" t="s">
+      <c r="B211" s="14" t="s">
         <v>328</v>
       </c>
       <c r="H211" t="s">
@@ -3628,7 +3668,7 @@
       </c>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B212" s="12" t="s">
+      <c r="B212" s="14" t="s">
         <v>329</v>
       </c>
       <c r="H212" t="s">
@@ -3636,7 +3676,7 @@
       </c>
     </row>
     <row r="213" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B213" s="12" t="s">
+      <c r="B213" s="14" t="s">
         <v>330</v>
       </c>
       <c r="H213" t="s">
@@ -3644,7 +3684,7 @@
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B214" s="12" t="s">
+      <c r="B214" s="14" t="s">
         <v>331</v>
       </c>
       <c r="H214" t="s">

</xml_diff>